<commit_message>
qa change actor names in text and figures, cap statements
</commit_message>
<xml_diff>
--- a/source/capstat_spreadsheets/DEQM_Capability_Statement_Producer_Client.xlsx
+++ b/source/capstat_spreadsheets/DEQM_Capability_Statement_Producer_Client.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\source\capstat_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6286871B-ABBA-415E-A3E4-2162BE94729D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EF35DE-8AEE-4680-8265-C37AB6C6F9C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" activeTab="4" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" activeTab="2" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
   <si>
     <t>Value</t>
   </si>
@@ -197,12 +197,6 @@
     <t>DeviceRequest</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/measure-deqm</t>
-  </si>
-  <si>
-    <t>Measure</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/medicationadministration-deqm</t>
   </si>
   <si>
@@ -215,9 +209,6 @@
     <t>MeasureReport</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/library-deqm</t>
-  </si>
-  <si>
     <t>Library</t>
   </si>
   <si>
@@ -266,15 +257,9 @@
     <t>DEQM DeviceRequest Profile</t>
   </si>
   <si>
-    <t>DEQM Measure Profile</t>
-  </si>
-  <si>
     <t>DEQM MedicationAdministration Profile</t>
   </si>
   <si>
-    <t>DEQM Library Profile</t>
-  </si>
-  <si>
     <t>DEQM Practitioner Profile</t>
   </si>
   <si>
@@ -306,9 +291,6 @@
   </si>
   <si>
     <t>QI Core</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/qicore/index.html</t>
   </si>
   <si>
     <t>This profile defines the expected capabilities of a Da Vinci DEQM Producer Client when conforming to the Da Vinci DEQM Implementation Guide. Producers include systems that are primary producers of patient healthcare information.  This CapabilityStatement resource includes the complete list of the *recommended*  Da Vinci DEQM profiles and RESTful operations that are  Da Vinci DEQM Producer Client could support. Clients have the option of choosing from this list based on their local use cases and other contextual requirements.</t>
@@ -347,19 +329,34 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/OperationDefinition/Measure-data-requirements</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/qicore/ImplementationGuide/qicore</t>
+  </si>
+  <si>
+    <t>CFQM</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/cqfmeasures/ImplementationGuide/cqfmeasures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF032F62"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -388,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -398,6 +395,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -745,7 +743,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +759,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -769,7 +767,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -787,15 +785,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0829A918-BBB6-6345-897C-371FBE4213DF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,15 +801,23 @@
         <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -821,10 +827,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B139EF60-0633-48C5-B394-C56F006BD6B3}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +860,7 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -868,7 +874,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -882,7 +888,7 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -893,16 +899,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,7 +916,7 @@
         <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -924,55 +930,55 @@
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,7 +986,7 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -994,41 +1000,13 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1088,21 +1066,21 @@
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1119,8 +1097,8 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,13 +1124,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1160,13 +1138,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1199,10 +1177,10 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1210,7 +1188,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,7 +1201,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>